<commit_message>
new to do list
</commit_message>
<xml_diff>
--- a/to_do_list.xlsx
+++ b/to_do_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\box-cert-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\L3\S2\box-cert-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DF7BE6-7854-4CA3-9F67-DF478FC053CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB1FE39-9033-4529-94D1-73643531EAF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="To do list" sheetId="6" r:id="rId1"/>
@@ -237,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -285,9 +285,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -341,11 +338,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp12.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$15" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$E$15" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp13.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$16" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$E$16" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp14.xml><?xml version="1.0" encoding="utf-8"?>
@@ -409,7 +406,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2378,7 +2375,7 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4" style="3" customWidth="1"/>
     <col min="2" max="2" width="10.08984375" style="9" customWidth="1"/>
@@ -2508,7 +2505,7 @@
         <v>5</v>
       </c>
       <c r="E8" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="12"/>
     </row>
@@ -2517,7 +2514,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="10"/>
-      <c r="C9" s="19" t="s">
+      <c r="C9" s="14" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="12" t="s">
@@ -2549,7 +2546,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="10"/>
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="19" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="12" t="s">
@@ -2620,7 +2617,7 @@
         <v>5</v>
       </c>
       <c r="E15" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="12"/>
     </row>
@@ -2636,7 +2633,7 @@
         <v>5</v>
       </c>
       <c r="E16" s="4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16" s="12"/>
     </row>
@@ -2804,7 +2801,7 @@
       <sortCondition descending="1" ref="D3:D28"/>
     </sortState>
   </autoFilter>
-  <conditionalFormatting sqref="A10:E11 A4:B9 D4:E9 A14:E28 A12:B13 D12:E13">
+  <conditionalFormatting sqref="A4:B9 D4:E9 A10:E11 A12:B13 D12:E13 A14:E28">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>AND($E4=TRUE,$C4&lt;&gt;"")</formula>
     </cfRule>

</xml_diff>